<commit_message>
Se modifica archivo gherkin en el escenario outline
</commit_message>
<xml_diff>
--- a/Gherkin.xlsx
+++ b/Gherkin.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Automatización de pruebas\Semana 5 y 6\Taller final\HomeSentry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Automatización de pruebas\Semana 5 y 6\Taller final\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74822E2A-98C5-4F21-A482-2445D61A43C4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3894A29-A563-420B-8BC7-9C7C803C16DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="139">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="140">
   <si>
     <t>Feature</t>
   </si>
@@ -637,6 +637,9 @@
   </si>
   <si>
     <t>podrá visualizar el nombre del producto &lt;Producto&gt; en el carro de compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precio </t>
   </si>
 </sst>
 </file>
@@ -797,18 +800,20 @@
     <xf numFmtId="49" fontId="8" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="11" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="12" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2259,7 +2264,7 @@
   <dimension ref="A1:F54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2274,602 +2279,655 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="20" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="20" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="20" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15"/>
-      <c r="F3" s="15"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="20"/>
+      <c r="E3" s="20"/>
+      <c r="F3" s="20"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="20" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15"/>
-      <c r="F4" s="15"/>
+      <c r="C4" s="20"/>
+      <c r="D4" s="20"/>
+      <c r="E4" s="20"/>
+      <c r="F4" s="20"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="20"/>
+      <c r="D5" s="20"/>
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="20"/>
+      <c r="D6" s="20"/>
+      <c r="E6" s="20"/>
+      <c r="F6" s="20"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
+      <c r="D7" s="20"/>
+      <c r="E7" s="20"/>
+      <c r="F7" s="20"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
+      <c r="C8" s="20"/>
+      <c r="D8" s="20"/>
+      <c r="E8" s="20"/>
+      <c r="F8" s="20"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20"/>
+      <c r="E9" s="20"/>
+      <c r="F9" s="20"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="20"/>
+      <c r="E10" s="20"/>
+      <c r="F10" s="20"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
+      <c r="C11" s="20"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="20"/>
+      <c r="F11" s="20"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="15"/>
-      <c r="F12" s="15"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="20"/>
+      <c r="F12" s="20"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="20"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="20"/>
+      <c r="F13" s="20"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="15"/>
+      <c r="B14" s="20"/>
+      <c r="C14" s="20"/>
+      <c r="D14" s="20"/>
+      <c r="E14" s="20"/>
+      <c r="F14" s="20"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="15"/>
+      <c r="C15" s="20"/>
+      <c r="D15" s="20"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="20"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
+      <c r="C16" s="20"/>
+      <c r="D16" s="20"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
+      <c r="C17" s="20"/>
+      <c r="D17" s="20"/>
+      <c r="E17" s="20"/>
+      <c r="F17" s="20"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
+      <c r="C18" s="20"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="20"/>
+      <c r="F18" s="20"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="20"/>
+      <c r="D19" s="20"/>
+      <c r="E19" s="20"/>
+      <c r="F19" s="20"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
+      <c r="B20" s="20"/>
+      <c r="C20" s="20"/>
+      <c r="D20" s="20"/>
+      <c r="E20" s="20"/>
+      <c r="F20" s="20"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
+      <c r="B21" s="20"/>
+      <c r="C21" s="20"/>
+      <c r="D21" s="20"/>
+      <c r="E21" s="20"/>
+      <c r="F21" s="20"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
+      <c r="C22" s="20"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="20"/>
+      <c r="F22" s="20"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="15"/>
-      <c r="E23" s="15"/>
-      <c r="F23" s="15"/>
+      <c r="C23" s="20"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="20"/>
+      <c r="F23" s="20"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="20" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="20"/>
+      <c r="E24" s="20"/>
+      <c r="F24" s="20"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="20" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="E26" s="20"/>
+      <c r="F26" s="20"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="20"/>
+      <c r="D28" s="20"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="20" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
+      <c r="C29" s="20"/>
+      <c r="D29" s="20"/>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="15"/>
-      <c r="F30" s="15"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="20" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
+      <c r="C31" s="20"/>
+      <c r="D31" s="20"/>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="20" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="15"/>
-      <c r="F32" s="15"/>
+      <c r="C32" s="20"/>
+      <c r="D32" s="20"/>
+      <c r="E32" s="20"/>
+      <c r="F32" s="20"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="15"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+      <c r="F33" s="20"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="15"/>
-      <c r="C34" s="15"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="15"/>
+      <c r="B34" s="20"/>
+      <c r="C34" s="20"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="20"/>
+      <c r="F34" s="20"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="15"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="20"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="20"/>
+      <c r="F35" s="20"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="20" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
+      <c r="C36" s="20"/>
+      <c r="D36" s="20"/>
+      <c r="E36" s="20"/>
+      <c r="F36" s="20"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="15"/>
-      <c r="E37" s="15"/>
-      <c r="F37" s="15"/>
+      <c r="C37" s="20"/>
+      <c r="D37" s="20"/>
+      <c r="E37" s="20"/>
+      <c r="F37" s="20"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="20" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="15"/>
-      <c r="F38" s="15"/>
+      <c r="C38" s="20"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+      <c r="F38" s="20"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="15"/>
-      <c r="D39" s="15"/>
-      <c r="E39" s="15"/>
-      <c r="F39" s="15"/>
+      <c r="C39" s="20"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+      <c r="F39" s="20"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="15"/>
-      <c r="F40" s="15"/>
+      <c r="B40" s="20"/>
+      <c r="C40" s="20"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="20"/>
+      <c r="F40" s="20"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="15"/>
-      <c r="F41" s="15"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="20"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="20"/>
+      <c r="F41" s="20"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15"/>
-      <c r="E42" s="15"/>
-      <c r="F42" s="15"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+      <c r="F42" s="20"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="15"/>
-      <c r="F43" s="15"/>
+      <c r="C43" s="20"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="20"/>
+      <c r="F43" s="20"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="20" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="15"/>
-      <c r="F44" s="15"/>
+      <c r="C44" s="20"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="20"/>
+      <c r="F44" s="20"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="20" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15"/>
-      <c r="E45" s="15"/>
-      <c r="F45" s="15"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+      <c r="F45" s="20"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="15"/>
-      <c r="F46" s="15"/>
+      <c r="B46" s="20"/>
+      <c r="C46" s="20"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+      <c r="F46" s="20"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="15"/>
-      <c r="F47" s="15"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="20"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="20"/>
+      <c r="F47" s="20"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="15"/>
-      <c r="F48" s="15"/>
+      <c r="B48" s="20"/>
+      <c r="C48" s="20"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="20"/>
+      <c r="F48" s="20"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="16" t="s">
+      <c r="A49" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="B49" s="17" t="s">
+      <c r="B49" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="18"/>
+      <c r="C49" s="21" t="s">
+        <v>139</v>
+      </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>
       <c r="F49" s="11"/>
     </row>
     <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="17" t="s">
         <v>132</v>
       </c>
-      <c r="B50" s="20">
+      <c r="B50" s="18">
         <v>1</v>
       </c>
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="18">
+        <v>250000</v>
+      </c>
+      <c r="D50" s="19" t="s">
         <v>121</v>
       </c>
-      <c r="D50" s="11"/>
       <c r="E50" s="11"/>
       <c r="F50" s="11"/>
     </row>
     <row r="51" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="17" t="s">
         <v>133</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="18">
         <v>1</v>
       </c>
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="18">
+        <v>110000</v>
+      </c>
+      <c r="D51" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="D51" s="11"/>
       <c r="E51" s="11"/>
       <c r="F51" s="11"/>
     </row>
     <row r="52" spans="1:6" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A52" s="19" t="s">
+      <c r="A52" s="17" t="s">
         <v>134</v>
       </c>
-      <c r="B52" s="20">
+      <c r="B52" s="18">
         <v>1</v>
       </c>
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="18">
+        <v>88000</v>
+      </c>
+      <c r="D52" s="19" t="s">
         <v>123</v>
       </c>
-      <c r="D52" s="11"/>
       <c r="E52" s="11"/>
       <c r="F52" s="11"/>
     </row>
     <row r="53" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A53" s="19" t="s">
+      <c r="A53" s="17" t="s">
         <v>135</v>
       </c>
-      <c r="B53" s="20">
+      <c r="B53" s="18">
         <v>1</v>
       </c>
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="18">
+        <v>150000</v>
+      </c>
+      <c r="D53" s="19" t="s">
         <v>124</v>
       </c>
-      <c r="D53" s="11"/>
       <c r="E53" s="11"/>
       <c r="F53" s="11"/>
     </row>
     <row r="54" spans="1:6" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="17" t="s">
         <v>136</v>
       </c>
-      <c r="B54" s="20">
+      <c r="B54" s="18">
         <v>3</v>
       </c>
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="18">
+        <v>210000</v>
+      </c>
+      <c r="D54" s="19" t="s">
         <v>125</v>
       </c>
-      <c r="D54" s="11"/>
       <c r="E54" s="11"/>
       <c r="F54" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="48">
+    <mergeCell ref="B12:F12"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+    <mergeCell ref="B4:F4"/>
+    <mergeCell ref="B5:F5"/>
+    <mergeCell ref="B6:F6"/>
+    <mergeCell ref="B7:F7"/>
+    <mergeCell ref="B8:F8"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="B10:F10"/>
+    <mergeCell ref="B11:F11"/>
+    <mergeCell ref="B24:F24"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="B14:F14"/>
+    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B16:F16"/>
+    <mergeCell ref="B17:F17"/>
+    <mergeCell ref="B18:F18"/>
+    <mergeCell ref="B19:F19"/>
+    <mergeCell ref="B20:F20"/>
+    <mergeCell ref="B21:F21"/>
+    <mergeCell ref="B22:F22"/>
+    <mergeCell ref="B23:F23"/>
+    <mergeCell ref="B36:F36"/>
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="B26:F26"/>
+    <mergeCell ref="B27:F27"/>
+    <mergeCell ref="B28:F28"/>
+    <mergeCell ref="B29:F29"/>
+    <mergeCell ref="B30:F30"/>
+    <mergeCell ref="B31:F31"/>
+    <mergeCell ref="B32:F32"/>
+    <mergeCell ref="B33:F33"/>
+    <mergeCell ref="B34:F34"/>
+    <mergeCell ref="B35:F35"/>
+    <mergeCell ref="B37:F37"/>
+    <mergeCell ref="B38:F38"/>
+    <mergeCell ref="B39:F39"/>
+    <mergeCell ref="B40:F40"/>
+    <mergeCell ref="B41:F41"/>
     <mergeCell ref="B48:F48"/>
     <mergeCell ref="B42:F42"/>
     <mergeCell ref="B43:F43"/>
@@ -2877,47 +2935,6 @@
     <mergeCell ref="B45:F45"/>
     <mergeCell ref="B46:F46"/>
     <mergeCell ref="B47:F47"/>
-    <mergeCell ref="B37:F37"/>
-    <mergeCell ref="B38:F38"/>
-    <mergeCell ref="B39:F39"/>
-    <mergeCell ref="B40:F40"/>
-    <mergeCell ref="B41:F41"/>
-    <mergeCell ref="B31:F31"/>
-    <mergeCell ref="B32:F32"/>
-    <mergeCell ref="B33:F33"/>
-    <mergeCell ref="B34:F34"/>
-    <mergeCell ref="B35:F35"/>
-    <mergeCell ref="B36:F36"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="B26:F26"/>
-    <mergeCell ref="B27:F27"/>
-    <mergeCell ref="B28:F28"/>
-    <mergeCell ref="B29:F29"/>
-    <mergeCell ref="B30:F30"/>
-    <mergeCell ref="B19:F19"/>
-    <mergeCell ref="B20:F20"/>
-    <mergeCell ref="B21:F21"/>
-    <mergeCell ref="B22:F22"/>
-    <mergeCell ref="B23:F23"/>
-    <mergeCell ref="B24:F24"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="B14:F14"/>
-    <mergeCell ref="B15:F15"/>
-    <mergeCell ref="B16:F16"/>
-    <mergeCell ref="B17:F17"/>
-    <mergeCell ref="B18:F18"/>
-    <mergeCell ref="B7:F7"/>
-    <mergeCell ref="B8:F8"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="B10:F10"/>
-    <mergeCell ref="B11:F11"/>
-    <mergeCell ref="B12:F12"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-    <mergeCell ref="B4:F4"/>
-    <mergeCell ref="B5:F5"/>
-    <mergeCell ref="B6:F6"/>
   </mergeCells>
   <printOptions horizontalCentered="1" gridLines="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Se agrega documento con  las evidencias de los casos de pruebas diseñados al 50%
</commit_message>
<xml_diff>
--- a/Gherkin.xlsx
+++ b/Gherkin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Automatización de pruebas\Semana 5 y 6\Taller final\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3894A29-A563-420B-8BC7-9C7C803C16DC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436D6E35-6F28-47B5-89DE-72D490FB32E0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicios - calculadora suma" sheetId="5" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="141">
   <si>
     <t>Feature</t>
   </si>
@@ -636,10 +636,13 @@
     <t xml:space="preserve">elige un electrodoméstico &lt;Producto&gt; con la cantidad &lt;Cantidad&gt; que desea de ese producto </t>
   </si>
   <si>
-    <t>podrá visualizar el nombre del producto &lt;Producto&gt; en el carro de compras</t>
-  </si>
-  <si>
     <t xml:space="preserve">Precio </t>
+  </si>
+  <si>
+    <t>podrá visualizar el nombre del producto &lt;Producto&gt; la cantidad &lt;Cantidad&gt; precio &lt;precio&gt; en el carro de compras</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deberá mostrar una respuesta 200 con resultado 0 </t>
   </si>
 </sst>
 </file>
@@ -809,11 +812,11 @@
     <xf numFmtId="49" fontId="13" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="49" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="14" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1283,8 +1286,8 @@
   </sheetPr>
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView topLeftCell="A7" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1531,7 +1534,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="B40" sqref="B40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1803,7 +1806,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>37</v>
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -1821,8 +1824,8 @@
   </sheetPr>
   <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2263,8 +2266,8 @@
   </sheetPr>
   <dimension ref="A1:F54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G50" sqref="G50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2279,517 +2282,517 @@
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="21" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="21" t="s">
         <v>94</v>
       </c>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="21"/>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5"/>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>98</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="21"/>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5"/>
-      <c r="B4" s="20" t="s">
+      <c r="B4" s="21" t="s">
         <v>99</v>
       </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="20"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="20"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
+      <c r="B5" s="21"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
     </row>
     <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
     </row>
     <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="20"/>
-      <c r="D7" s="20"/>
-      <c r="E7" s="20"/>
-      <c r="F7" s="20"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
     </row>
     <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="C8" s="20"/>
-      <c r="D8" s="20"/>
-      <c r="E8" s="20"/>
-      <c r="F8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
     </row>
     <row r="9" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B9" s="20" t="s">
+      <c r="B9" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C9" s="20"/>
-      <c r="D9" s="20"/>
-      <c r="E9" s="20"/>
-      <c r="F9" s="20"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="21" t="s">
         <v>108</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="20"/>
-      <c r="E10" s="20"/>
-      <c r="F10" s="20"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21"/>
     </row>
     <row r="11" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B11" s="20" t="s">
+      <c r="B11" s="21" t="s">
         <v>104</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="20"/>
-      <c r="F11" s="20"/>
+      <c r="C11" s="21"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21"/>
     </row>
     <row r="12" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
-      <c r="B12" s="20"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="20"/>
-      <c r="F12" s="20"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
     </row>
     <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="20"/>
-      <c r="C13" s="20"/>
-      <c r="D13" s="20"/>
-      <c r="E13" s="20"/>
-      <c r="F13" s="20"/>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21"/>
     </row>
     <row r="14" spans="1:6" ht="15" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
-      <c r="D14" s="20"/>
-      <c r="E14" s="20"/>
-      <c r="F14" s="20"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="21"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
     </row>
     <row r="15" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B15" s="20" t="s">
+      <c r="B15" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="20"/>
-      <c r="E15" s="20"/>
-      <c r="F15" s="20"/>
+      <c r="C15" s="21"/>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
     </row>
     <row r="16" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="20"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21"/>
     </row>
     <row r="17" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="20" t="s">
+      <c r="B17" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="20"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="20"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="21" t="s">
         <v>110</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="20"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="20"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11"/>
-      <c r="B19" s="20"/>
-      <c r="C19" s="20"/>
-      <c r="D19" s="20"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="20"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
     </row>
     <row r="20" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B20" s="20"/>
-      <c r="C20" s="20"/>
-      <c r="D20" s="20"/>
-      <c r="E20" s="20"/>
-      <c r="F20" s="20"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
     </row>
     <row r="21" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="20"/>
-      <c r="C21" s="20"/>
-      <c r="D21" s="20"/>
-      <c r="E21" s="20"/>
-      <c r="F21" s="20"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="21" t="s">
         <v>111</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
     </row>
     <row r="23" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B23" s="20" t="s">
+      <c r="B23" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="20"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
     </row>
     <row r="24" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="20" t="s">
+      <c r="B24" s="21" t="s">
         <v>112</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="20"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
     </row>
     <row r="25" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
     </row>
     <row r="26" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
-      <c r="B26" s="20"/>
-      <c r="C26" s="20"/>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
     </row>
     <row r="27" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="B27" s="20"/>
-      <c r="C27" s="20"/>
-      <c r="D27" s="20"/>
-      <c r="E27" s="20"/>
-      <c r="F27" s="20"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
     </row>
     <row r="28" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B28" s="20"/>
-      <c r="C28" s="20"/>
-      <c r="D28" s="20"/>
-      <c r="E28" s="20"/>
-      <c r="F28" s="20"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
     </row>
     <row r="29" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B29" s="20" t="s">
+      <c r="B29" s="21" t="s">
         <v>115</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="20"/>
-      <c r="F29" s="20"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
     </row>
     <row r="30" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B30" s="20" t="s">
+      <c r="B30" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="20"/>
-      <c r="F30" s="20"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
     </row>
     <row r="31" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B31" s="20" t="s">
+      <c r="B31" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="20"/>
-      <c r="E31" s="20"/>
-      <c r="F31" s="20"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
     </row>
     <row r="32" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B32" s="20" t="s">
+      <c r="B32" s="21" t="s">
         <v>117</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="20"/>
-      <c r="E32" s="20"/>
-      <c r="F32" s="20"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11"/>
-      <c r="B33" s="20"/>
-      <c r="C33" s="20"/>
-      <c r="D33" s="20"/>
-      <c r="E33" s="20"/>
-      <c r="F33" s="20"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
     </row>
     <row r="34" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="B34" s="20"/>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
     </row>
     <row r="35" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B35" s="20"/>
-      <c r="C35" s="20"/>
-      <c r="D35" s="20"/>
-      <c r="E35" s="20"/>
-      <c r="F35" s="20"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
     </row>
     <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B36" s="20" t="s">
+      <c r="B36" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="20"/>
-      <c r="E36" s="20"/>
-      <c r="F36" s="20"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
     </row>
     <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B37" s="20" t="s">
+      <c r="B37" s="21" t="s">
         <v>102</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="20"/>
-      <c r="E37" s="20"/>
-      <c r="F37" s="20"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
     </row>
     <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="20" t="s">
+      <c r="B38" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="20"/>
-      <c r="E38" s="20"/>
-      <c r="F38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
     </row>
     <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B39" s="20" t="s">
+      <c r="B39" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="E39" s="20"/>
-      <c r="F39" s="20"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
     </row>
     <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
-      <c r="B40" s="20"/>
-      <c r="C40" s="20"/>
-      <c r="D40" s="20"/>
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
     </row>
     <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="20"/>
-      <c r="C41" s="20"/>
-      <c r="D41" s="20"/>
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="21" t="s">
         <v>105</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="20"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
     </row>
     <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="21" t="s">
         <v>137</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
     </row>
     <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B45" s="20" t="s">
-        <v>138</v>
-      </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
+      <c r="B45" s="21" t="s">
+        <v>139</v>
+      </c>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
     </row>
     <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
-      <c r="B46" s="20"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
     </row>
     <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="14" t="s">
         <v>127</v>
       </c>
-      <c r="B47" s="20"/>
-      <c r="C47" s="20"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
     </row>
     <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11"/>
-      <c r="B48" s="20"/>
-      <c r="C48" s="20"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
     </row>
     <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
@@ -2798,8 +2801,8 @@
       <c r="B49" s="16" t="s">
         <v>131</v>
       </c>
-      <c r="C49" s="21" t="s">
-        <v>139</v>
+      <c r="C49" s="20" t="s">
+        <v>138</v>
       </c>
       <c r="D49" s="11"/>
       <c r="E49" s="11"/>

</xml_diff>